<commit_message>
add sample details file information
</commit_message>
<xml_diff>
--- a/Load/ontology/Microbiome/doc/Microbiome_terms_mappings.xlsx
+++ b/Load/ontology/Microbiome/doc/Microbiome_terms_mappings.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/VEuPathDB-git/ApiCommonData/Load/ontology/Microbiome/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06854B1-76B8-D146-BF99-164619A6C837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CC1EC9-7B43-F847-B6E0-3DB6D85988D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1060" windowWidth="26580" windowHeight="14860" xr2:uid="{E0296402-9AB9-CD44-A13E-78A419041986}"/>
+    <workbookView xWindow="6720" yWindow="680" windowWidth="26580" windowHeight="14860" xr2:uid="{E0296402-9AB9-CD44-A13E-78A419041986}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleDetails_ontologyTerms" sheetId="3" r:id="rId1"/>
     <sheet name="microbiome.owl" sheetId="5" r:id="rId2"/>
     <sheet name="ontology term not used" sheetId="7" r:id="rId3"/>
     <sheet name="ontologyMappingsMicrobiome.xml" sheetId="4" r:id="rId4"/>
+    <sheet name="SampleDetails_files" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13888" uniqueCount="2156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13940" uniqueCount="2158">
   <si>
     <t>body_site</t>
   </si>
@@ -6498,6 +6499,12 @@
   </si>
   <si>
     <t>EDA</t>
+  </si>
+  <si>
+    <t>Dataset (based on sample details file)</t>
+  </si>
+  <si>
+    <t>Category (based on host)</t>
   </si>
 </sst>
 </file>
@@ -6907,7 +6914,7 @@
   <dimension ref="A1:M793"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H770" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H598" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="K779" sqref="K779:K793"/>
@@ -52365,4 +52372,230 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39604157-289C-6A45-8FF5-8FEB263B9580}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>2156</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>254</v>
+      </c>
+      <c r="B16" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>257</v>
+      </c>
+      <c r="B17" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>258</v>
+      </c>
+      <c r="B18" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>287</v>
+      </c>
+      <c r="B19" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>290</v>
+      </c>
+      <c r="B20" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>328</v>
+      </c>
+      <c r="B21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>330</v>
+      </c>
+      <c r="B22" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>385</v>
+      </c>
+      <c r="B23" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>386</v>
+      </c>
+      <c r="B24" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>173</v>
+      </c>
+      <c r="B25" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" t="s">
+        <v>400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>